<commit_message>
Commit updated Iselin Nov 2016 Winkler data
</commit_message>
<xml_diff>
--- a/PHORCYS/data/processed/Iselin_WHOI_2016_11/Iselin_WHOI_2016_11_Winklers_workup.xlsx
+++ b/PHORCYS/data/processed/Iselin_WHOI_2016_11/Iselin_WHOI_2016_11_Winklers_workup.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28100" yWindow="540" windowWidth="37180" windowHeight="18140" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="110816" sheetId="1" r:id="rId1"/>
     <sheet name="110916" sheetId="2" r:id="rId2"/>
     <sheet name="111016" sheetId="3" r:id="rId3"/>
     <sheet name="111116" sheetId="4" r:id="rId4"/>
-    <sheet name="Aggregated_with_timepoints" sheetId="5" r:id="rId5"/>
+    <sheet name="111416" sheetId="6" r:id="rId5"/>
+    <sheet name="Aggregated_with_timepoints" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="117">
   <si>
     <t>Phorcys</t>
   </si>
@@ -370,6 +371,18 @@
   </si>
   <si>
     <t>O2_final_umol_L_dark_se</t>
+  </si>
+  <si>
+    <t>L29</t>
+  </si>
+  <si>
+    <t>L30</t>
+  </si>
+  <si>
+    <t>L31</t>
+  </si>
+  <si>
+    <t>L32</t>
   </si>
 </sst>
 </file>
@@ -3257,7 +3270,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="I1" sqref="I1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4153,10 +4166,615 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6.1130000000000004</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <f>E2*1.42903</f>
+        <v>8.7356603900000014</v>
+      </c>
+      <c r="J2">
+        <f>I2*1000/32.01</f>
+        <v>272.90410465479545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.1719999999999997</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="0">E3*1.42903</f>
+        <v>8.81997316</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J17" si="1">I3*1000/32.01</f>
+        <v>275.5380556076226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6.048</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>8.6427734400000009</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>270.00229428303658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6.3239999999999998</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>9.0371857200000001</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>282.32382755388943</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(J2:J5)</f>
+        <v>275.19207052483603</v>
+      </c>
+      <c r="L5">
+        <f>STDEV(J2:J5)</f>
+        <v>5.2646693236258129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6.1479999999999997</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>8.7856764399999996</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>274.46661793189628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.1639999999999997</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>8.8085409200000004</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>275.18090971571388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6.1870000000000003</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>8.8414086100000002</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>276.20770415495161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.1719999999999997</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>8.81997316</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>275.5380556076226</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE(J6:J9)</f>
+        <v>275.34832185254606</v>
+      </c>
+      <c r="L9">
+        <f>STDEV(J6:J9)</f>
+        <v>0.72571010436932804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.2949999999999999</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>8.9957438500000002</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>281.02917369572015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6.35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>9.0743404999999999</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>283.48455170259297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6.2960000000000003</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>8.9971728800000008</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>281.07381693220873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6.3029999999999999</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>9.0071760899999997</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>281.38631958762886</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE(J10:J13)</f>
+        <v>281.74346547953769</v>
+      </c>
+      <c r="L13">
+        <f>STDEV(J10:J13)</f>
+        <v>1.1715483136415783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>6.3179999999999996</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>9.02861154</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>282.05596813495782</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6.532</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>9.3344239600000005</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>291.60962074351767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6.2850000000000001</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>8.9814535500000012</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>280.58274133083421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6.3179999999999996</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>9.02861154</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>282.05596813495782</v>
+      </c>
+      <c r="K17">
+        <f>AVERAGE(J14:J17)</f>
+        <v>284.07607458606691</v>
+      </c>
+      <c r="L17">
+        <f>STDEV(J14:J17)</f>
+        <v>5.0701530248498043</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4333,7 +4951,7 @@
         <v>2.4796479401033027</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K8" si="2">(G3-C3)/(B3-A3)</f>
+        <f t="shared" ref="K3:K7" si="2">(G3-C3)/(B3-A3)</f>
         <v>0.7469156874037165</v>
       </c>
       <c r="L3">
@@ -4692,15 +5310,79 @@
         <f>'111116'!L21/SQRT(4)</f>
         <v>2.3357843049892453</v>
       </c>
+      <c r="E9">
+        <f>'111416'!K9</f>
+        <v>275.34832185254606</v>
+      </c>
+      <c r="F9">
+        <f>'111416'!L9/SQRT(4)</f>
+        <v>0.36285505218466402</v>
+      </c>
+      <c r="G9">
+        <f>'111416'!K5</f>
+        <v>275.19207052483603</v>
+      </c>
+      <c r="H9">
+        <f>'111416'!L5/SQRT(4)</f>
+        <v>2.6323346618129064</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9" si="8">(E9-C9)/(B9-A9)</f>
+        <v>-14.949686400595779</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9" si="9">SQRT(SUM(F9^2+D9^2))/(B9-A9)</f>
+        <v>5.5257670586468564</v>
+      </c>
+      <c r="K9">
+        <f>(G9-C9)/(B9-A9)</f>
+        <v>-15.314949244589267</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9" si="10">SQRT(SUM(H9^2+D9^2))/(B9-A9)</f>
+        <v>8.2268027474347836</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9" si="11">-K9</f>
+        <v>15.314949244589267</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9" si="12">L9</f>
+        <v>8.2268027474347836</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9" si="13">I9</f>
+        <v>-14.949686400595779</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9" si="14">J9</f>
+        <v>5.5257670586468564</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>98</v>
       </c>
+      <c r="C10">
+        <f>'111416'!K13</f>
+        <v>281.74346547953769</v>
+      </c>
+      <c r="D10">
+        <f>'111416'!L13/SQRT(4)</f>
+        <v>0.58577415682078915</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>99</v>
+      </c>
+      <c r="C11">
+        <f>'111416'!K17</f>
+        <v>284.07607458606691</v>
+      </c>
+      <c r="D11">
+        <f>'111416'!L17/SQRT(4)</f>
+        <v>2.5350765124249022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>